<commit_message>
new version of attributable warming figure
</commit_message>
<xml_diff>
--- a/current_methods_statistics_250818TrueCount.xlsx
+++ b/current_methods_statistics_250818TrueCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JohnMatthew/Downloads/Thorne_15_codefigurestats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B83E7548-B7AA-FF45-BE45-C807796CEF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E51E178-68E5-3349-A0FF-EC13C13E8EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{DF6C84C7-2CCE-2F4B-BE9F-E0FC9C65B259}"/>
+    <workbookView xWindow="17420" yWindow="4600" windowWidth="27640" windowHeight="16940" xr2:uid="{DF6C84C7-2CCE-2F4B-BE9F-E0FC9C65B259}"/>
   </bookViews>
   <sheets>
     <sheet name="current_methods_statistics_2508" sheetId="1" r:id="rId1"/>
@@ -1204,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DB77BF-4242-8242-9DFF-9681B038B3BF}">
   <dimension ref="A1:V69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="L59" sqref="L59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5741,7 +5741,7 @@
         <v>32</v>
       </c>
       <c r="C68" s="2" t="str">
-        <f t="shared" ref="C68:C70" ca="1" si="3">IF(ISNUMBER(D68),SUM(INDIRECT(_xlfn.CONCAT("N",ROW(),":N",ROW()+D68-1))),"")</f>
+        <f t="shared" ref="C68:C69" ca="1" si="3">IF(ISNUMBER(D68),SUM(INDIRECT(_xlfn.CONCAT("N",ROW(),":N",ROW()+D68-1))),"")</f>
         <v/>
       </c>
       <c r="E68" t="s">

</xml_diff>